<commit_message>
Corrigir conversão de datas do Excel (formato serial)
</commit_message>
<xml_diff>
--- a/carteira-export.xlsx
+++ b/carteira-export.xlsx
@@ -607,14 +607,22 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="4" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -622,9 +630,7 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
-      <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1101,7 +1107,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1232,7 +1238,7 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4">
@@ -2165,107 +2171,107 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="D31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K31" s="1" t="s">
+      <c r="H31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="D32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K32" s="1" t="s">
+      <c r="H32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K33" s="1" t="s">
+      <c r="H33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2985,7 +2991,7 @@
       <c r="E54" t="s">
         <v>157</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F54" s="3">
         <v>23850.77</v>
       </c>
       <c r="G54" t="s">
@@ -3145,7 +3151,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="s">
+      <c r="A59" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B59" t="s">
@@ -3180,7 +3186,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="s">
+      <c r="A60" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B60" t="s">
@@ -3215,7 +3221,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="s">
+      <c r="A61" s="4" t="s">
         <v>170</v>
       </c>
       <c r="B61" t="s">
@@ -3250,7 +3256,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="s">
+      <c r="A62" s="4" t="s">
         <v>170</v>
       </c>
       <c r="B62" t="s">
@@ -3285,185 +3291,185 @@
       </c>
     </row>
     <row r="63" ht="14.25">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="G63" s="1" t="s">
+      <c r="G63" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K63" s="1" t="s">
+      <c r="H63" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K63" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="64" ht="14.25">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E64" s="1" t="s">
+      <c r="D64" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="G64" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" s="3" customFormat="1" ht="14.25">
-      <c r="A65" s="4" t="s">
+      <c r="H64" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" s="1" customFormat="1" ht="14.25">
+      <c r="A65" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E65" s="4">
+      <c r="E65" s="7">
         <v>24</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F65" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="G65" s="4" t="s">
+      <c r="G65" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H65" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K65" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" s="3" customFormat="1" ht="14.25">
-      <c r="A66" s="5">
+      <c r="H65" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J65" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K65" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" s="1" customFormat="1" ht="14.25">
+      <c r="A66" s="6">
         <v>45971</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E66" s="4">
+      <c r="E66" s="7">
         <v>12</v>
       </c>
-      <c r="F66" s="4">
+      <c r="F66" s="7">
         <v>40.520000000000003</v>
       </c>
-      <c r="G66" s="4" t="s">
+      <c r="G66" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H66" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I66" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J66" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K66" s="4" t="s">
+      <c r="H66" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J66" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K66" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="67" ht="14.25">
-      <c r="A67" s="5">
+      <c r="A67" s="6">
         <v>45971</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E67" s="4">
+      <c r="E67" s="7">
         <v>12</v>
       </c>
-      <c r="F67" s="4">
+      <c r="F67" s="7">
         <v>42.200000000000003</v>
       </c>
-      <c r="G67" s="4" t="s">
+      <c r="G67" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H67" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I67" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J67" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K67" s="4" t="s">
+      <c r="H67" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J67" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K67" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="68" ht="14.25">
-      <c r="A68" s="6">
+      <c r="A68" s="8">
         <v>45974</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="7" t="s">
         <v>120</v>
       </c>
       <c r="C68" t="s">
@@ -3478,68 +3484,68 @@
       <c r="F68">
         <v>122.40000000000001</v>
       </c>
-      <c r="G68" s="4" t="s">
+      <c r="G68" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H68" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I68" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J68" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K68" s="4" t="s">
+      <c r="H68" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J68" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K68" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="69" ht="14.25">
-      <c r="A69" s="6">
+      <c r="A69" s="8">
         <v>45973</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E69" s="7">
+      <c r="E69" s="9">
         <v>60</v>
       </c>
-      <c r="F69" s="7">
+      <c r="F69" s="9">
         <v>18.34</v>
       </c>
-      <c r="G69" s="4" t="s">
+      <c r="G69" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H69" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I69" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J69" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K69" s="4" t="s">
+      <c r="H69" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J69" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K69" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="70" ht="14.25">
-      <c r="A70" s="6">
+      <c r="A70" s="8">
         <v>45974</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="7" t="s">
         <v>180</v>
       </c>
       <c r="C70" t="s">
         <v>181</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E70">
@@ -3548,33 +3554,33 @@
       <c r="F70">
         <v>23.289999999999999</v>
       </c>
-      <c r="G70" s="4" t="s">
+      <c r="G70" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H70" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I70" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K70" s="4" t="s">
+      <c r="H70" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I70" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J70" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K70" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="71" ht="14.25">
-      <c r="A71" s="6">
+      <c r="A71" s="8">
         <v>45974</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C71" t="s">
         <v>39</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D71" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E71">
@@ -3583,24 +3589,24 @@
       <c r="F71">
         <v>35.649999999999999</v>
       </c>
-      <c r="G71" s="4" t="s">
+      <c r="G71" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H71" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I71" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J71" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K71" s="4" t="s">
+      <c r="H71" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J71" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K71" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="72" ht="14.25">
-      <c r="A72" s="6">
+      <c r="A72" s="8">
         <v>45972</v>
       </c>
       <c r="B72" t="s">
@@ -3609,7 +3615,7 @@
       <c r="C72" t="s">
         <v>182</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E72">
@@ -3618,24 +3624,24 @@
       <c r="F72">
         <v>88.599999999999994</v>
       </c>
-      <c r="G72" s="4" t="s">
+      <c r="G72" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H72" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I72" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K72" s="4" t="s">
+      <c r="H72" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J72" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K72" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="73" ht="14.25">
-      <c r="A73" s="6">
+      <c r="A73" s="8">
         <v>45971</v>
       </c>
       <c r="B73" t="s">
@@ -3650,57 +3656,57 @@
       <c r="E73">
         <v>3.5006000000000002e-004</v>
       </c>
-      <c r="F73" s="2">
+      <c r="F73" s="3">
         <v>504123.97999999998</v>
       </c>
       <c r="G73" t="s">
         <v>184</v>
       </c>
-      <c r="H73" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I73" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K73" s="4" t="s">
+      <c r="H73" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J73" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K73" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="74" ht="14.25">
-      <c r="A74" s="6">
+      <c r="A74" s="8">
         <v>45975</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E74" s="1">
+      <c r="D74" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E74" s="2">
         <v>3.8890000000000002e-004</v>
       </c>
-      <c r="F74" s="2">
+      <c r="F74" s="3">
         <v>566759.97999999998</v>
       </c>
       <c r="G74" t="s">
         <v>184</v>
       </c>
-      <c r="H74" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I74" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J74" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K74" s="4" t="s">
+      <c r="H74" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I74" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J74" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K74" s="7" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>